<commit_message>
vaja 10 - dokoncano razen dodatne naloge
</commit_message>
<xml_diff>
--- a/10-razpredelnice/poraba.xlsx
+++ b/10-razpredelnice/poraba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katja/Versioned/Predmeti/racunalniski-praktikum/vaje/03-excel/vaje2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kajab\Documents\racunalniski-praktikum\10-razpredelnice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB024210-1BD4-674C-B304-48B62DBB35CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE0354-D0C6-47A1-9DBC-22414EC732FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="-26560" windowWidth="23020" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Poraba" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Poraba!$B$2:$G$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId2"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Bencin</t>
   </si>
@@ -78,13 +81,44 @@
   <si>
     <t>Prikaz</t>
   </si>
+  <si>
+    <t>Oznake stolpcev</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Povprečje od Poraba</t>
+  </si>
+  <si>
+    <t>Vsota od Prevoženo</t>
+  </si>
+  <si>
+    <t>Vrednosti</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000\ &quot;€/l&quot;"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-424]_-;\-* #,##0.00\ [$€-424]_-;_-* &quot;-&quot;??\ [$€-424]_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,18 +156,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -189,7 +235,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="172" formatCode="d/mm/yy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFEBF1DE"/>
@@ -239,7 +285,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -257,13 +303,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-424]_-;\-* #,##0.00\ [$€-424]_-;_-* &quot;-&quot;??\ [$€-424]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="172" formatCode="d/mm/yy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -276,6 +322,1123 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kaja Bartelj" refreshedDate="45631.675714351855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{A7F56C61-6971-407D-BE21-F2BCA08B7C22}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="realna_poraba_cupra__2"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="Datum" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-05-05T00:00:00" maxDate="2023-10-15T00:00:00" count="19">
+        <d v="2023-05-05T00:00:00"/>
+        <d v="2023-05-13T00:00:00"/>
+        <d v="2023-05-22T00:00:00"/>
+        <d v="2023-05-27T00:00:00"/>
+        <d v="2023-06-08T00:00:00"/>
+        <d v="2023-06-16T00:00:00"/>
+        <d v="2023-06-22T00:00:00"/>
+        <d v="2023-07-06T00:00:00"/>
+        <d v="2023-07-15T00:00:00"/>
+        <d v="2023-07-22T00:00:00"/>
+        <d v="2023-07-31T00:00:00"/>
+        <d v="2023-08-13T00:00:00"/>
+        <d v="2023-08-25T00:00:00"/>
+        <d v="2023-09-06T00:00:00"/>
+        <d v="2023-09-15T00:00:00"/>
+        <d v="2023-09-22T00:00:00"/>
+        <d v="2023-09-29T00:00:00"/>
+        <d v="2023-10-06T00:00:00"/>
+        <d v="2023-10-14T00:00:00"/>
+      </sharedItems>
+      <fieldGroup par="8"/>
+    </cacheField>
+    <cacheField name="Litri" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="34.04" maxValue="43.1"/>
+    </cacheField>
+    <cacheField name="Plačano" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="47.043279999999996" maxValue="64.097279999999998"/>
+    </cacheField>
+    <cacheField name="Števec" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="41907" maxValue="52176"/>
+    </cacheField>
+    <cacheField name="Prevoženo" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="446" maxValue="683"/>
+    </cacheField>
+    <cacheField name="Poraba" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="6.3103953147877023" maxValue="8.1008968609865484"/>
+    </cacheField>
+    <cacheField name="Prikaz" numFmtId="2">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="6.3103953147877023" maxValue="8.1008968609865484"/>
+    </cacheField>
+    <cacheField name="Dnevi (Datum)" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="days" startDate="2023-05-05T00:00:00" endDate="2023-10-15T00:00:00"/>
+        <groupItems count="368">
+          <s v="&lt;05/05/2023"/>
+          <s v="01-Jan"/>
+          <s v="02-Jan"/>
+          <s v="03-Jan"/>
+          <s v="04-Jan"/>
+          <s v="05-Jan"/>
+          <s v="06-Jan"/>
+          <s v="07-Jan"/>
+          <s v="08-Jan"/>
+          <s v="09-Jan"/>
+          <s v="10-Jan"/>
+          <s v="11-Jan"/>
+          <s v="12-Jan"/>
+          <s v="13-Jan"/>
+          <s v="14-Jan"/>
+          <s v="15-Jan"/>
+          <s v="16-Jan"/>
+          <s v="17-Jan"/>
+          <s v="18-Jan"/>
+          <s v="19-Jan"/>
+          <s v="20-Jan"/>
+          <s v="21-Jan"/>
+          <s v="22-Jan"/>
+          <s v="23-Jan"/>
+          <s v="24-Jan"/>
+          <s v="25-Jan"/>
+          <s v="26-Jan"/>
+          <s v="27-Jan"/>
+          <s v="28-Jan"/>
+          <s v="29-Jan"/>
+          <s v="30-Jan"/>
+          <s v="31-Jan"/>
+          <s v="01-Feb"/>
+          <s v="02-Feb"/>
+          <s v="03-Feb"/>
+          <s v="04-Feb"/>
+          <s v="05-Feb"/>
+          <s v="06-Feb"/>
+          <s v="07-Feb"/>
+          <s v="08-Feb"/>
+          <s v="09-Feb"/>
+          <s v="10-Feb"/>
+          <s v="11-Feb"/>
+          <s v="12-Feb"/>
+          <s v="13-Feb"/>
+          <s v="14-Feb"/>
+          <s v="15-Feb"/>
+          <s v="16-Feb"/>
+          <s v="17-Feb"/>
+          <s v="18-Feb"/>
+          <s v="19-Feb"/>
+          <s v="20-Feb"/>
+          <s v="21-Feb"/>
+          <s v="22-Feb"/>
+          <s v="23-Feb"/>
+          <s v="24-Feb"/>
+          <s v="25-Feb"/>
+          <s v="26-Feb"/>
+          <s v="27-Feb"/>
+          <s v="28-Feb"/>
+          <s v="29-Feb"/>
+          <s v="01-Mar"/>
+          <s v="02-Mar"/>
+          <s v="03-Mar"/>
+          <s v="04-Mar"/>
+          <s v="05-Mar"/>
+          <s v="06-Mar"/>
+          <s v="07-Mar"/>
+          <s v="08-Mar"/>
+          <s v="09-Mar"/>
+          <s v="10-Mar"/>
+          <s v="11-Mar"/>
+          <s v="12-Mar"/>
+          <s v="13-Mar"/>
+          <s v="14-Mar"/>
+          <s v="15-Mar"/>
+          <s v="16-Mar"/>
+          <s v="17-Mar"/>
+          <s v="18-Mar"/>
+          <s v="19-Mar"/>
+          <s v="20-Mar"/>
+          <s v="21-Mar"/>
+          <s v="22-Mar"/>
+          <s v="23-Mar"/>
+          <s v="24-Mar"/>
+          <s v="25-Mar"/>
+          <s v="26-Mar"/>
+          <s v="27-Mar"/>
+          <s v="28-Mar"/>
+          <s v="29-Mar"/>
+          <s v="30-Mar"/>
+          <s v="31-Mar"/>
+          <s v="01-Apr"/>
+          <s v="02-Apr"/>
+          <s v="03-Apr"/>
+          <s v="04-Apr"/>
+          <s v="05-Apr"/>
+          <s v="06-Apr"/>
+          <s v="07-Apr"/>
+          <s v="08-Apr"/>
+          <s v="09-Apr"/>
+          <s v="10-Apr"/>
+          <s v="11-Apr"/>
+          <s v="12-Apr"/>
+          <s v="13-Apr"/>
+          <s v="14-Apr"/>
+          <s v="15-Apr"/>
+          <s v="16-Apr"/>
+          <s v="17-Apr"/>
+          <s v="18-Apr"/>
+          <s v="19-Apr"/>
+          <s v="20-Apr"/>
+          <s v="21-Apr"/>
+          <s v="22-Apr"/>
+          <s v="23-Apr"/>
+          <s v="24-Apr"/>
+          <s v="25-Apr"/>
+          <s v="26-Apr"/>
+          <s v="27-Apr"/>
+          <s v="28-Apr"/>
+          <s v="29-Apr"/>
+          <s v="30-Apr"/>
+          <s v="01-May"/>
+          <s v="02-May"/>
+          <s v="03-May"/>
+          <s v="04-May"/>
+          <s v="05-May"/>
+          <s v="06-May"/>
+          <s v="07-May"/>
+          <s v="08-May"/>
+          <s v="09-May"/>
+          <s v="10-May"/>
+          <s v="11-May"/>
+          <s v="12-May"/>
+          <s v="13-May"/>
+          <s v="14-May"/>
+          <s v="15-May"/>
+          <s v="16-May"/>
+          <s v="17-May"/>
+          <s v="18-May"/>
+          <s v="19-May"/>
+          <s v="20-May"/>
+          <s v="21-May"/>
+          <s v="22-May"/>
+          <s v="23-May"/>
+          <s v="24-May"/>
+          <s v="25-May"/>
+          <s v="26-May"/>
+          <s v="27-May"/>
+          <s v="28-May"/>
+          <s v="29-May"/>
+          <s v="30-May"/>
+          <s v="31-May"/>
+          <s v="01-Jun"/>
+          <s v="02-Jun"/>
+          <s v="03-Jun"/>
+          <s v="04-Jun"/>
+          <s v="05-Jun"/>
+          <s v="06-Jun"/>
+          <s v="07-Jun"/>
+          <s v="08-Jun"/>
+          <s v="09-Jun"/>
+          <s v="10-Jun"/>
+          <s v="11-Jun"/>
+          <s v="12-Jun"/>
+          <s v="13-Jun"/>
+          <s v="14-Jun"/>
+          <s v="15-Jun"/>
+          <s v="16-Jun"/>
+          <s v="17-Jun"/>
+          <s v="18-Jun"/>
+          <s v="19-Jun"/>
+          <s v="20-Jun"/>
+          <s v="21-Jun"/>
+          <s v="22-Jun"/>
+          <s v="23-Jun"/>
+          <s v="24-Jun"/>
+          <s v="25-Jun"/>
+          <s v="26-Jun"/>
+          <s v="27-Jun"/>
+          <s v="28-Jun"/>
+          <s v="29-Jun"/>
+          <s v="30-Jun"/>
+          <s v="01-Jul"/>
+          <s v="02-Jul"/>
+          <s v="03-Jul"/>
+          <s v="04-Jul"/>
+          <s v="05-Jul"/>
+          <s v="06-Jul"/>
+          <s v="07-Jul"/>
+          <s v="08-Jul"/>
+          <s v="09-Jul"/>
+          <s v="10-Jul"/>
+          <s v="11-Jul"/>
+          <s v="12-Jul"/>
+          <s v="13-Jul"/>
+          <s v="14-Jul"/>
+          <s v="15-Jul"/>
+          <s v="16-Jul"/>
+          <s v="17-Jul"/>
+          <s v="18-Jul"/>
+          <s v="19-Jul"/>
+          <s v="20-Jul"/>
+          <s v="21-Jul"/>
+          <s v="22-Jul"/>
+          <s v="23-Jul"/>
+          <s v="24-Jul"/>
+          <s v="25-Jul"/>
+          <s v="26-Jul"/>
+          <s v="27-Jul"/>
+          <s v="28-Jul"/>
+          <s v="29-Jul"/>
+          <s v="30-Jul"/>
+          <s v="31-Jul"/>
+          <s v="01-Aug"/>
+          <s v="02-Aug"/>
+          <s v="03-Aug"/>
+          <s v="04-Aug"/>
+          <s v="05-Aug"/>
+          <s v="06-Aug"/>
+          <s v="07-Aug"/>
+          <s v="08-Aug"/>
+          <s v="09-Aug"/>
+          <s v="10-Aug"/>
+          <s v="11-Aug"/>
+          <s v="12-Aug"/>
+          <s v="13-Aug"/>
+          <s v="14-Aug"/>
+          <s v="15-Aug"/>
+          <s v="16-Aug"/>
+          <s v="17-Aug"/>
+          <s v="18-Aug"/>
+          <s v="19-Aug"/>
+          <s v="20-Aug"/>
+          <s v="21-Aug"/>
+          <s v="22-Aug"/>
+          <s v="23-Aug"/>
+          <s v="24-Aug"/>
+          <s v="25-Aug"/>
+          <s v="26-Aug"/>
+          <s v="27-Aug"/>
+          <s v="28-Aug"/>
+          <s v="29-Aug"/>
+          <s v="30-Aug"/>
+          <s v="31-Aug"/>
+          <s v="01-Sep"/>
+          <s v="02-Sep"/>
+          <s v="03-Sep"/>
+          <s v="04-Sep"/>
+          <s v="05-Sep"/>
+          <s v="06-Sep"/>
+          <s v="07-Sep"/>
+          <s v="08-Sep"/>
+          <s v="09-Sep"/>
+          <s v="10-Sep"/>
+          <s v="11-Sep"/>
+          <s v="12-Sep"/>
+          <s v="13-Sep"/>
+          <s v="14-Sep"/>
+          <s v="15-Sep"/>
+          <s v="16-Sep"/>
+          <s v="17-Sep"/>
+          <s v="18-Sep"/>
+          <s v="19-Sep"/>
+          <s v="20-Sep"/>
+          <s v="21-Sep"/>
+          <s v="22-Sep"/>
+          <s v="23-Sep"/>
+          <s v="24-Sep"/>
+          <s v="25-Sep"/>
+          <s v="26-Sep"/>
+          <s v="27-Sep"/>
+          <s v="28-Sep"/>
+          <s v="29-Sep"/>
+          <s v="30-Sep"/>
+          <s v="01-Oct"/>
+          <s v="02-Oct"/>
+          <s v="03-Oct"/>
+          <s v="04-Oct"/>
+          <s v="05-Oct"/>
+          <s v="06-Oct"/>
+          <s v="07-Oct"/>
+          <s v="08-Oct"/>
+          <s v="09-Oct"/>
+          <s v="10-Oct"/>
+          <s v="11-Oct"/>
+          <s v="12-Oct"/>
+          <s v="13-Oct"/>
+          <s v="14-Oct"/>
+          <s v="15-Oct"/>
+          <s v="16-Oct"/>
+          <s v="17-Oct"/>
+          <s v="18-Oct"/>
+          <s v="19-Oct"/>
+          <s v="20-Oct"/>
+          <s v="21-Oct"/>
+          <s v="22-Oct"/>
+          <s v="23-Oct"/>
+          <s v="24-Oct"/>
+          <s v="25-Oct"/>
+          <s v="26-Oct"/>
+          <s v="27-Oct"/>
+          <s v="28-Oct"/>
+          <s v="29-Oct"/>
+          <s v="30-Oct"/>
+          <s v="31-Oct"/>
+          <s v="01-Nov"/>
+          <s v="02-Nov"/>
+          <s v="03-Nov"/>
+          <s v="04-Nov"/>
+          <s v="05-Nov"/>
+          <s v="06-Nov"/>
+          <s v="07-Nov"/>
+          <s v="08-Nov"/>
+          <s v="09-Nov"/>
+          <s v="10-Nov"/>
+          <s v="11-Nov"/>
+          <s v="12-Nov"/>
+          <s v="13-Nov"/>
+          <s v="14-Nov"/>
+          <s v="15-Nov"/>
+          <s v="16-Nov"/>
+          <s v="17-Nov"/>
+          <s v="18-Nov"/>
+          <s v="19-Nov"/>
+          <s v="20-Nov"/>
+          <s v="21-Nov"/>
+          <s v="22-Nov"/>
+          <s v="23-Nov"/>
+          <s v="24-Nov"/>
+          <s v="25-Nov"/>
+          <s v="26-Nov"/>
+          <s v="27-Nov"/>
+          <s v="28-Nov"/>
+          <s v="29-Nov"/>
+          <s v="30-Nov"/>
+          <s v="01-Dec"/>
+          <s v="02-Dec"/>
+          <s v="03-Dec"/>
+          <s v="04-Dec"/>
+          <s v="05-Dec"/>
+          <s v="06-Dec"/>
+          <s v="07-Dec"/>
+          <s v="08-Dec"/>
+          <s v="09-Dec"/>
+          <s v="10-Dec"/>
+          <s v="11-Dec"/>
+          <s v="12-Dec"/>
+          <s v="13-Dec"/>
+          <s v="14-Dec"/>
+          <s v="15-Dec"/>
+          <s v="16-Dec"/>
+          <s v="17-Dec"/>
+          <s v="18-Dec"/>
+          <s v="19-Dec"/>
+          <s v="20-Dec"/>
+          <s v="21-Dec"/>
+          <s v="22-Dec"/>
+          <s v="23-Dec"/>
+          <s v="24-Dec"/>
+          <s v="25-Dec"/>
+          <s v="26-Dec"/>
+          <s v="27-Dec"/>
+          <s v="28-Dec"/>
+          <s v="29-Dec"/>
+          <s v="30-Dec"/>
+          <s v="31-Dec"/>
+          <s v="&gt;15/10/2023"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Meseci (Datum)" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="months" startDate="2023-05-05T00:00:00" endDate="2023-10-15T00:00:00"/>
+        <groupItems count="14">
+          <s v="&lt;05/05/2023"/>
+          <s v="Jan"/>
+          <s v="Feb"/>
+          <s v="Mar"/>
+          <s v="Apr"/>
+          <s v="May"/>
+          <s v="Jun"/>
+          <s v="Jul"/>
+          <s v="Aug"/>
+          <s v="Sep"/>
+          <s v="Oct"/>
+          <s v="Nov"/>
+          <s v="Dec"/>
+          <s v="&gt;15/10/2023"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="19">
+  <r>
+    <x v="0"/>
+    <n v="41.17"/>
+    <n v="58.296720000000001"/>
+    <n v="41907"/>
+    <s v=""/>
+    <s v=""/>
+    <e v="#VALUE!"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="43.02"/>
+    <n v="59.797800000000002"/>
+    <n v="42521"/>
+    <n v="614"/>
+    <n v="7.006514657980456"/>
+    <n v="7.006514657980456"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="41.67"/>
+    <n v="57.921299999999995"/>
+    <n v="43181"/>
+    <n v="660"/>
+    <n v="6.3136363636363644"/>
+    <n v="6.3136363636363644"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="34.04"/>
+    <n v="47.043279999999996"/>
+    <n v="43696"/>
+    <n v="515"/>
+    <n v="6.6097087378640769"/>
+    <n v="6.6097087378640769"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="42.42"/>
+    <n v="59.897039999999997"/>
+    <n v="44314"/>
+    <n v="618"/>
+    <n v="6.8640776699029127"/>
+    <n v="6.8640776699029127"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="43.1"/>
+    <n v="60.857199999999999"/>
+    <n v="44997"/>
+    <n v="683"/>
+    <n v="6.3103953147877023"/>
+    <n v="6.3103953147877023"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="38.18"/>
+    <n v="54.368319999999997"/>
+    <n v="45546"/>
+    <n v="549"/>
+    <n v="6.9544626593806917"/>
+    <n v="6.9544626593806917"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="40.659999999999997"/>
+    <n v="58.713039999999992"/>
+    <n v="46126"/>
+    <n v="580"/>
+    <n v="7.0103448275862066"/>
+    <n v="7.0103448275862066"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="39.17"/>
+    <n v="56.561480000000003"/>
+    <n v="46687"/>
+    <n v="561"/>
+    <n v="6.9821746880570412"/>
+    <n v="6.9821746880570412"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="40.29"/>
+    <n v="58.662239999999997"/>
+    <n v="47250"/>
+    <n v="563"/>
+    <n v="7.1563055062166967"/>
+    <n v="7.1563055062166967"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="41.01"/>
+    <n v="59.710559999999994"/>
+    <n v="47867"/>
+    <n v="617"/>
+    <n v="6.6466774716369521"/>
+    <n v="6.6466774716369521"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="37.18"/>
+    <n v="56.178979999999996"/>
+    <n v="48407"/>
+    <n v="540"/>
+    <n v="6.8851851851851844"/>
+    <n v="6.8851851851851844"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="41.46"/>
+    <n v="62.646059999999999"/>
+    <n v="49005"/>
+    <n v="598"/>
+    <n v="6.9331103678929766"/>
+    <n v="6.9331103678929766"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="35.97"/>
+    <n v="55.537680000000002"/>
+    <n v="49480"/>
+    <n v="475"/>
+    <n v="7.5726315789473686"/>
+    <n v="7.5726315789473686"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="38.74"/>
+    <n v="60.085740000000001"/>
+    <n v="50012"/>
+    <n v="532"/>
+    <n v="7.2819548872180455"/>
+    <n v="7.2819548872180455"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="36.130000000000003"/>
+    <n v="56.03763"/>
+    <n v="50458"/>
+    <n v="446"/>
+    <n v="8.1008968609865484"/>
+    <n v="8.1008968609865484"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="38.51"/>
+    <n v="61.153880000000001"/>
+    <n v="50991"/>
+    <n v="533"/>
+    <n v="7.2251407129455911"/>
+    <n v="7.2251407129455911"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="38.840000000000003"/>
+    <n v="61.677920000000007"/>
+    <n v="51593"/>
+    <n v="602"/>
+    <n v="6.4518272425249172"/>
+    <n v="6.4518272425249172"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="41.73"/>
+    <n v="64.097279999999998"/>
+    <n v="52176"/>
+    <n v="583"/>
+    <n v="7.1578044596912509"/>
+    <n v="7.1578044596912509"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64FCA948-F978-45AE-BCAB-F5155804EE62}" name="Vrtilna tabela2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Vrednosti" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B27:H30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="14" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="369">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item sd="0" x="26"/>
+        <item sd="0" x="27"/>
+        <item sd="0" x="28"/>
+        <item sd="0" x="29"/>
+        <item sd="0" x="30"/>
+        <item sd="0" x="31"/>
+        <item sd="0" x="32"/>
+        <item sd="0" x="33"/>
+        <item sd="0" x="34"/>
+        <item sd="0" x="35"/>
+        <item sd="0" x="36"/>
+        <item sd="0" x="37"/>
+        <item sd="0" x="38"/>
+        <item sd="0" x="39"/>
+        <item sd="0" x="40"/>
+        <item sd="0" x="41"/>
+        <item sd="0" x="42"/>
+        <item sd="0" x="43"/>
+        <item sd="0" x="44"/>
+        <item sd="0" x="45"/>
+        <item sd="0" x="46"/>
+        <item sd="0" x="47"/>
+        <item sd="0" x="48"/>
+        <item sd="0" x="49"/>
+        <item sd="0" x="50"/>
+        <item sd="0" x="51"/>
+        <item sd="0" x="52"/>
+        <item sd="0" x="53"/>
+        <item sd="0" x="54"/>
+        <item sd="0" x="55"/>
+        <item sd="0" x="56"/>
+        <item sd="0" x="57"/>
+        <item sd="0" x="58"/>
+        <item sd="0" x="59"/>
+        <item sd="0" x="60"/>
+        <item sd="0" x="61"/>
+        <item sd="0" x="62"/>
+        <item sd="0" x="63"/>
+        <item sd="0" x="64"/>
+        <item sd="0" x="65"/>
+        <item sd="0" x="66"/>
+        <item sd="0" x="67"/>
+        <item sd="0" x="68"/>
+        <item sd="0" x="69"/>
+        <item sd="0" x="70"/>
+        <item sd="0" x="71"/>
+        <item sd="0" x="72"/>
+        <item sd="0" x="73"/>
+        <item sd="0" x="74"/>
+        <item sd="0" x="75"/>
+        <item sd="0" x="76"/>
+        <item sd="0" x="77"/>
+        <item sd="0" x="78"/>
+        <item sd="0" x="79"/>
+        <item sd="0" x="80"/>
+        <item sd="0" x="81"/>
+        <item sd="0" x="82"/>
+        <item sd="0" x="83"/>
+        <item sd="0" x="84"/>
+        <item sd="0" x="85"/>
+        <item sd="0" x="86"/>
+        <item sd="0" x="87"/>
+        <item sd="0" x="88"/>
+        <item sd="0" x="89"/>
+        <item sd="0" x="90"/>
+        <item sd="0" x="91"/>
+        <item sd="0" x="92"/>
+        <item sd="0" x="93"/>
+        <item sd="0" x="94"/>
+        <item sd="0" x="95"/>
+        <item sd="0" x="96"/>
+        <item sd="0" x="97"/>
+        <item sd="0" x="98"/>
+        <item sd="0" x="99"/>
+        <item sd="0" x="100"/>
+        <item sd="0" x="101"/>
+        <item sd="0" x="102"/>
+        <item sd="0" x="103"/>
+        <item sd="0" x="104"/>
+        <item sd="0" x="105"/>
+        <item sd="0" x="106"/>
+        <item sd="0" x="107"/>
+        <item sd="0" x="108"/>
+        <item sd="0" x="109"/>
+        <item sd="0" x="110"/>
+        <item sd="0" x="111"/>
+        <item sd="0" x="112"/>
+        <item sd="0" x="113"/>
+        <item sd="0" x="114"/>
+        <item sd="0" x="115"/>
+        <item sd="0" x="116"/>
+        <item sd="0" x="117"/>
+        <item sd="0" x="118"/>
+        <item sd="0" x="119"/>
+        <item sd="0" x="120"/>
+        <item sd="0" x="121"/>
+        <item sd="0" x="122"/>
+        <item sd="0" x="123"/>
+        <item sd="0" x="124"/>
+        <item sd="0" x="125"/>
+        <item sd="0" x="126"/>
+        <item sd="0" x="127"/>
+        <item sd="0" x="128"/>
+        <item sd="0" x="129"/>
+        <item sd="0" x="130"/>
+        <item sd="0" x="131"/>
+        <item sd="0" x="132"/>
+        <item sd="0" x="133"/>
+        <item sd="0" x="134"/>
+        <item sd="0" x="135"/>
+        <item sd="0" x="136"/>
+        <item sd="0" x="137"/>
+        <item sd="0" x="138"/>
+        <item sd="0" x="139"/>
+        <item sd="0" x="140"/>
+        <item sd="0" x="141"/>
+        <item sd="0" x="142"/>
+        <item sd="0" x="143"/>
+        <item sd="0" x="144"/>
+        <item sd="0" x="145"/>
+        <item sd="0" x="146"/>
+        <item sd="0" x="147"/>
+        <item sd="0" x="148"/>
+        <item sd="0" x="149"/>
+        <item sd="0" x="150"/>
+        <item sd="0" x="151"/>
+        <item sd="0" x="152"/>
+        <item sd="0" x="153"/>
+        <item sd="0" x="154"/>
+        <item sd="0" x="155"/>
+        <item sd="0" x="156"/>
+        <item sd="0" x="157"/>
+        <item sd="0" x="158"/>
+        <item sd="0" x="159"/>
+        <item sd="0" x="160"/>
+        <item sd="0" x="161"/>
+        <item sd="0" x="162"/>
+        <item sd="0" x="163"/>
+        <item sd="0" x="164"/>
+        <item sd="0" x="165"/>
+        <item sd="0" x="166"/>
+        <item sd="0" x="167"/>
+        <item sd="0" x="168"/>
+        <item sd="0" x="169"/>
+        <item sd="0" x="170"/>
+        <item sd="0" x="171"/>
+        <item sd="0" x="172"/>
+        <item sd="0" x="173"/>
+        <item sd="0" x="174"/>
+        <item sd="0" x="175"/>
+        <item sd="0" x="176"/>
+        <item sd="0" x="177"/>
+        <item sd="0" x="178"/>
+        <item sd="0" x="179"/>
+        <item sd="0" x="180"/>
+        <item sd="0" x="181"/>
+        <item sd="0" x="182"/>
+        <item sd="0" x="183"/>
+        <item sd="0" x="184"/>
+        <item sd="0" x="185"/>
+        <item sd="0" x="186"/>
+        <item sd="0" x="187"/>
+        <item sd="0" x="188"/>
+        <item sd="0" x="189"/>
+        <item sd="0" x="190"/>
+        <item sd="0" x="191"/>
+        <item sd="0" x="192"/>
+        <item sd="0" x="193"/>
+        <item sd="0" x="194"/>
+        <item sd="0" x="195"/>
+        <item sd="0" x="196"/>
+        <item sd="0" x="197"/>
+        <item sd="0" x="198"/>
+        <item sd="0" x="199"/>
+        <item sd="0" x="200"/>
+        <item sd="0" x="201"/>
+        <item sd="0" x="202"/>
+        <item sd="0" x="203"/>
+        <item sd="0" x="204"/>
+        <item sd="0" x="205"/>
+        <item sd="0" x="206"/>
+        <item sd="0" x="207"/>
+        <item sd="0" x="208"/>
+        <item sd="0" x="209"/>
+        <item sd="0" x="210"/>
+        <item sd="0" x="211"/>
+        <item sd="0" x="212"/>
+        <item sd="0" x="213"/>
+        <item sd="0" x="214"/>
+        <item sd="0" x="215"/>
+        <item sd="0" x="216"/>
+        <item sd="0" x="217"/>
+        <item sd="0" x="218"/>
+        <item sd="0" x="219"/>
+        <item sd="0" x="220"/>
+        <item sd="0" x="221"/>
+        <item sd="0" x="222"/>
+        <item sd="0" x="223"/>
+        <item sd="0" x="224"/>
+        <item sd="0" x="225"/>
+        <item sd="0" x="226"/>
+        <item sd="0" x="227"/>
+        <item sd="0" x="228"/>
+        <item sd="0" x="229"/>
+        <item sd="0" x="230"/>
+        <item sd="0" x="231"/>
+        <item sd="0" x="232"/>
+        <item sd="0" x="233"/>
+        <item sd="0" x="234"/>
+        <item sd="0" x="235"/>
+        <item sd="0" x="236"/>
+        <item sd="0" x="237"/>
+        <item sd="0" x="238"/>
+        <item sd="0" x="239"/>
+        <item sd="0" x="240"/>
+        <item sd="0" x="241"/>
+        <item sd="0" x="242"/>
+        <item sd="0" x="243"/>
+        <item sd="0" x="244"/>
+        <item sd="0" x="245"/>
+        <item sd="0" x="246"/>
+        <item sd="0" x="247"/>
+        <item sd="0" x="248"/>
+        <item sd="0" x="249"/>
+        <item sd="0" x="250"/>
+        <item sd="0" x="251"/>
+        <item sd="0" x="252"/>
+        <item sd="0" x="253"/>
+        <item sd="0" x="254"/>
+        <item sd="0" x="255"/>
+        <item sd="0" x="256"/>
+        <item sd="0" x="257"/>
+        <item sd="0" x="258"/>
+        <item sd="0" x="259"/>
+        <item sd="0" x="260"/>
+        <item sd="0" x="261"/>
+        <item sd="0" x="262"/>
+        <item sd="0" x="263"/>
+        <item sd="0" x="264"/>
+        <item sd="0" x="265"/>
+        <item sd="0" x="266"/>
+        <item sd="0" x="267"/>
+        <item sd="0" x="268"/>
+        <item sd="0" x="269"/>
+        <item sd="0" x="270"/>
+        <item sd="0" x="271"/>
+        <item sd="0" x="272"/>
+        <item sd="0" x="273"/>
+        <item sd="0" x="274"/>
+        <item sd="0" x="275"/>
+        <item sd="0" x="276"/>
+        <item sd="0" x="277"/>
+        <item sd="0" x="278"/>
+        <item sd="0" x="279"/>
+        <item sd="0" x="280"/>
+        <item sd="0" x="281"/>
+        <item sd="0" x="282"/>
+        <item sd="0" x="283"/>
+        <item sd="0" x="284"/>
+        <item sd="0" x="285"/>
+        <item sd="0" x="286"/>
+        <item sd="0" x="287"/>
+        <item sd="0" x="288"/>
+        <item sd="0" x="289"/>
+        <item sd="0" x="290"/>
+        <item sd="0" x="291"/>
+        <item sd="0" x="292"/>
+        <item sd="0" x="293"/>
+        <item sd="0" x="294"/>
+        <item sd="0" x="295"/>
+        <item sd="0" x="296"/>
+        <item sd="0" x="297"/>
+        <item sd="0" x="298"/>
+        <item sd="0" x="299"/>
+        <item sd="0" x="300"/>
+        <item sd="0" x="301"/>
+        <item sd="0" x="302"/>
+        <item sd="0" x="303"/>
+        <item sd="0" x="304"/>
+        <item sd="0" x="305"/>
+        <item sd="0" x="306"/>
+        <item sd="0" x="307"/>
+        <item sd="0" x="308"/>
+        <item sd="0" x="309"/>
+        <item sd="0" x="310"/>
+        <item sd="0" x="311"/>
+        <item sd="0" x="312"/>
+        <item sd="0" x="313"/>
+        <item sd="0" x="314"/>
+        <item sd="0" x="315"/>
+        <item sd="0" x="316"/>
+        <item sd="0" x="317"/>
+        <item sd="0" x="318"/>
+        <item sd="0" x="319"/>
+        <item sd="0" x="320"/>
+        <item sd="0" x="321"/>
+        <item sd="0" x="322"/>
+        <item sd="0" x="323"/>
+        <item sd="0" x="324"/>
+        <item sd="0" x="325"/>
+        <item sd="0" x="326"/>
+        <item sd="0" x="327"/>
+        <item sd="0" x="328"/>
+        <item sd="0" x="329"/>
+        <item sd="0" x="330"/>
+        <item sd="0" x="331"/>
+        <item sd="0" x="332"/>
+        <item sd="0" x="333"/>
+        <item sd="0" x="334"/>
+        <item sd="0" x="335"/>
+        <item sd="0" x="336"/>
+        <item sd="0" x="337"/>
+        <item sd="0" x="338"/>
+        <item sd="0" x="339"/>
+        <item sd="0" x="340"/>
+        <item sd="0" x="341"/>
+        <item sd="0" x="342"/>
+        <item sd="0" x="343"/>
+        <item sd="0" x="344"/>
+        <item sd="0" x="345"/>
+        <item sd="0" x="346"/>
+        <item sd="0" x="347"/>
+        <item sd="0" x="348"/>
+        <item sd="0" x="349"/>
+        <item sd="0" x="350"/>
+        <item sd="0" x="351"/>
+        <item sd="0" x="352"/>
+        <item sd="0" x="353"/>
+        <item sd="0" x="354"/>
+        <item sd="0" x="355"/>
+        <item sd="0" x="356"/>
+        <item sd="0" x="357"/>
+        <item sd="0" x="358"/>
+        <item sd="0" x="359"/>
+        <item sd="0" x="360"/>
+        <item sd="0" x="361"/>
+        <item sd="0" x="362"/>
+        <item sd="0" x="363"/>
+        <item sd="0" x="364"/>
+        <item sd="0" x="365"/>
+        <item sd="0" x="366"/>
+        <item sd="0" x="367"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="8"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Vsota od Prevoženo" fld="4" baseField="8" baseItem="0"/>
+    <dataField name="Povprečje od Poraba" fld="5" subtotal="average" baseField="8" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -300,16 +1463,24 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4B308AD5-65CF-A249-80D4-A2A1301BDB4E}" name="realna_poraba_cupra__2" displayName="realna_poraba_cupra__2" ref="B2:H21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="B2:H21" xr:uid="{4B308AD5-65CF-A249-80D4-A2A1301BDB4E}"/>
+  <autoFilter ref="B2:H21" xr:uid="{4B308AD5-65CF-A249-80D4-A2A1301BDB4E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E4C5B71E-FC31-5C41-A064-103F27749A97}" uniqueName="1" name="Datum" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6DC2697C-FCB3-8A47-945B-8CD05834AA8C}" uniqueName="2" name="Litri" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{19DBC541-3ADF-4E48-8786-6E42DA219788}" uniqueName="3" name="Plačano" queryTableFieldId="3" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3238A9AD-2FC0-0E49-9EE3-7019C05B366B}" uniqueName="4" name="Števec" queryTableFieldId="4" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{E0B5480D-9C8F-CA4C-941D-AE9FDE0CDFDC}" uniqueName="5" name="Prevoženo" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{1DEAFC6B-8470-6742-BAB3-957B7429D133}" uniqueName="6" name="Poraba" queryTableFieldId="6" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{911769A8-5CFE-8245-A64B-38797D90A3B5}" uniqueName="11" name="Prikaz" queryTableFieldId="11" dataDxfId="5">
-      <calculatedColumnFormula>realna_poraba_cupra__2[[#This Row],[Poraba]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{E4C5B71E-FC31-5C41-A064-103F27749A97}" uniqueName="1" name="Datum" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6DC2697C-FCB3-8A47-945B-8CD05834AA8C}" uniqueName="2" name="Litri" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{19DBC541-3ADF-4E48-8786-6E42DA219788}" uniqueName="3" name="Plačano" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{3238A9AD-2FC0-0E49-9EE3-7019C05B366B}" uniqueName="4" name="Števec" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{E0B5480D-9C8F-CA4C-941D-AE9FDE0CDFDC}" uniqueName="5" name="Prevoženo" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{1DEAFC6B-8470-6742-BAB3-957B7429D133}" uniqueName="6" name="Poraba" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{911769A8-5CFE-8245-A64B-38797D90A3B5}" uniqueName="11" name="Prikaz" queryTableFieldId="11" dataDxfId="7">
+      <calculatedColumnFormula>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -317,14 +1488,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8D6AF57-84FE-3944-82AB-DB7DC1C050CB}" name="Table3" displayName="Table3" ref="J2:K25" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="J2:K25" xr:uid="{E8D6AF57-84FE-3944-82AB-DB7DC1C050CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8D6AF57-84FE-3944-82AB-DB7DC1C050CB}" name="Table3" displayName="Table3" ref="J2:K25" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="J2:K25" xr:uid="{E8D6AF57-84FE-3944-82AB-DB7DC1C050CB}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J3:K25">
     <sortCondition ref="J2:J25"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0C7E1327-9FA7-3E43-8151-18CCECA1E09D}" name="Veljavnost" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{079EA12A-47EB-F54A-8E37-30D8BCE75150}" name="Bencin" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0C7E1327-9FA7-3E43-8151-18CCECA1E09D}" name="Veljavnost" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{079EA12A-47EB-F54A-8E37-30D8BCE75150}" name="Bencin" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -617,28 +1791,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CECC9D-4E93-D44D-AE31-BECED325B0FB}">
-  <dimension ref="B2:K29"/>
+  <dimension ref="B2:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -667,13 +1840,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>45051</v>
       </c>
       <c r="C3" s="3">
         <v>41.17</v>
       </c>
+      <c r="D3" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>58.296720000000001</v>
+      </c>
       <c r="E3" s="2">
         <v>41907</v>
       </c>
@@ -683,6 +1860,10 @@
       <c r="G3" t="s">
         <v>4</v>
       </c>
+      <c r="H3" s="3" t="e">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="J3" s="1">
         <v>44930</v>
       </c>
@@ -690,16 +1871,32 @@
         <v>1.276</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>45059</v>
       </c>
       <c r="C4" s="3">
         <v>43.02</v>
       </c>
+      <c r="D4" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>59.797800000000002</v>
+      </c>
       <c r="E4" s="2">
         <v>42521</v>
       </c>
+      <c r="F4" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E3</f>
+        <v>614</v>
+      </c>
+      <c r="G4" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.006514657980456</v>
+      </c>
+      <c r="H4" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.006514657980456</v>
+      </c>
       <c r="J4" s="1">
         <v>44943</v>
       </c>
@@ -707,16 +1904,32 @@
         <v>1.288</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>45068</v>
       </c>
       <c r="C5" s="3">
         <v>41.67</v>
       </c>
+      <c r="D5" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>57.921299999999995</v>
+      </c>
       <c r="E5" s="2">
         <v>43181</v>
       </c>
+      <c r="F5" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E4</f>
+        <v>660</v>
+      </c>
+      <c r="G5" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.3136363636363644</v>
+      </c>
+      <c r="H5" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.3136363636363644</v>
+      </c>
       <c r="J5" s="1">
         <v>44957</v>
       </c>
@@ -724,16 +1937,32 @@
         <v>1.355</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>45073</v>
       </c>
       <c r="C6" s="3">
         <v>34.04</v>
       </c>
+      <c r="D6" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>47.043279999999996</v>
+      </c>
       <c r="E6" s="2">
         <v>43696</v>
       </c>
+      <c r="F6" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E5</f>
+        <v>515</v>
+      </c>
+      <c r="G6" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.6097087378640769</v>
+      </c>
+      <c r="H6" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.6097087378640769</v>
+      </c>
       <c r="J6" s="1">
         <v>44971</v>
       </c>
@@ -741,16 +1970,32 @@
         <v>1.355</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>45085</v>
       </c>
       <c r="C7" s="3">
         <v>42.42</v>
       </c>
+      <c r="D7" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>59.897039999999997</v>
+      </c>
       <c r="E7" s="2">
         <v>44314</v>
       </c>
+      <c r="F7" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E6</f>
+        <v>618</v>
+      </c>
+      <c r="G7" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.8640776699029127</v>
+      </c>
+      <c r="H7" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.8640776699029127</v>
+      </c>
       <c r="J7" s="1">
         <v>44985</v>
       </c>
@@ -758,16 +2003,32 @@
         <v>1.359</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>45093</v>
       </c>
       <c r="C8" s="3">
         <v>43.1</v>
       </c>
+      <c r="D8" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>60.857199999999999</v>
+      </c>
       <c r="E8" s="2">
         <v>44997</v>
       </c>
+      <c r="F8" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E7</f>
+        <v>683</v>
+      </c>
+      <c r="G8" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.3103953147877023</v>
+      </c>
+      <c r="H8" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.3103953147877023</v>
+      </c>
       <c r="J8" s="1">
         <v>44999</v>
       </c>
@@ -775,16 +2036,32 @@
         <v>1.3740000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>45099</v>
       </c>
       <c r="C9" s="3">
         <v>38.18</v>
       </c>
+      <c r="D9" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>54.368319999999997</v>
+      </c>
       <c r="E9" s="2">
         <v>45546</v>
       </c>
+      <c r="F9" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E8</f>
+        <v>549</v>
+      </c>
+      <c r="G9" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9544626593806917</v>
+      </c>
+      <c r="H9" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9544626593806917</v>
+      </c>
       <c r="J9" s="1">
         <v>45013</v>
       </c>
@@ -792,16 +2069,32 @@
         <v>1.3740000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>45113</v>
       </c>
       <c r="C10" s="3">
         <v>40.659999999999997</v>
       </c>
+      <c r="D10" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>58.713039999999992</v>
+      </c>
       <c r="E10" s="2">
         <v>46126</v>
       </c>
+      <c r="F10" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E9</f>
+        <v>580</v>
+      </c>
+      <c r="G10" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.0103448275862066</v>
+      </c>
+      <c r="H10" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.0103448275862066</v>
+      </c>
       <c r="J10" s="1">
         <v>45028</v>
       </c>
@@ -809,16 +2102,32 @@
         <v>1.4159999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>45122</v>
       </c>
       <c r="C11" s="3">
         <v>39.17</v>
       </c>
+      <c r="D11" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>56.561480000000003</v>
+      </c>
       <c r="E11" s="2">
         <v>46687</v>
       </c>
+      <c r="F11" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E10</f>
+        <v>561</v>
+      </c>
+      <c r="G11" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9821746880570412</v>
+      </c>
+      <c r="H11" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9821746880570412</v>
+      </c>
       <c r="J11" s="1">
         <v>45041</v>
       </c>
@@ -826,16 +2135,32 @@
         <v>1.4159999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>45129</v>
       </c>
       <c r="C12" s="3">
         <v>40.29</v>
       </c>
+      <c r="D12" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>58.662239999999997</v>
+      </c>
       <c r="E12" s="2">
         <v>47250</v>
       </c>
+      <c r="F12" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E11</f>
+        <v>563</v>
+      </c>
+      <c r="G12" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.1563055062166967</v>
+      </c>
+      <c r="H12" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.1563055062166967</v>
+      </c>
       <c r="J12" s="1">
         <v>45055</v>
       </c>
@@ -843,16 +2168,32 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>45138</v>
       </c>
       <c r="C13" s="3">
         <v>41.01</v>
       </c>
+      <c r="D13" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>59.710559999999994</v>
+      </c>
       <c r="E13" s="2">
         <v>47867</v>
       </c>
+      <c r="F13" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E12</f>
+        <v>617</v>
+      </c>
+      <c r="G13" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.6466774716369521</v>
+      </c>
+      <c r="H13" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.6466774716369521</v>
+      </c>
       <c r="J13" s="1">
         <v>45069</v>
       </c>
@@ -860,16 +2201,32 @@
         <v>1.3819999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>45151</v>
       </c>
       <c r="C14" s="3">
         <v>37.18</v>
       </c>
+      <c r="D14" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>56.178979999999996</v>
+      </c>
       <c r="E14" s="2">
         <v>48407</v>
       </c>
+      <c r="F14" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E13</f>
+        <v>540</v>
+      </c>
+      <c r="G14" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.8851851851851844</v>
+      </c>
+      <c r="H14" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.8851851851851844</v>
+      </c>
       <c r="J14" s="1">
         <v>45083</v>
       </c>
@@ -877,16 +2234,32 @@
         <v>1.4119999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>45163</v>
       </c>
       <c r="C15" s="3">
         <v>41.46</v>
       </c>
+      <c r="D15" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>62.646059999999999</v>
+      </c>
       <c r="E15" s="2">
         <v>49005</v>
       </c>
+      <c r="F15" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E14</f>
+        <v>598</v>
+      </c>
+      <c r="G15" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9331103678929766</v>
+      </c>
+      <c r="H15" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.9331103678929766</v>
+      </c>
       <c r="J15" s="1">
         <v>45097</v>
       </c>
@@ -894,16 +2267,32 @@
         <v>1.4239999999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>45175</v>
       </c>
       <c r="C16" s="3">
         <v>35.97</v>
       </c>
+      <c r="D16" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>55.537680000000002</v>
+      </c>
       <c r="E16" s="2">
         <v>49480</v>
       </c>
+      <c r="F16" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E15</f>
+        <v>475</v>
+      </c>
+      <c r="G16" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.5726315789473686</v>
+      </c>
+      <c r="H16" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.5726315789473686</v>
+      </c>
       <c r="J16" s="1">
         <v>45111</v>
       </c>
@@ -911,16 +2300,32 @@
         <v>1.444</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>45184</v>
       </c>
       <c r="C17" s="3">
         <v>38.74</v>
       </c>
+      <c r="D17" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>60.085740000000001</v>
+      </c>
       <c r="E17" s="2">
         <v>50012</v>
       </c>
+      <c r="F17" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E16</f>
+        <v>532</v>
+      </c>
+      <c r="G17" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.2819548872180455</v>
+      </c>
+      <c r="H17" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.2819548872180455</v>
+      </c>
       <c r="J17" s="1">
         <v>45125</v>
       </c>
@@ -928,16 +2333,32 @@
         <v>1.456</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>45191</v>
       </c>
       <c r="C18" s="3">
         <v>36.130000000000003</v>
       </c>
+      <c r="D18" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>56.03763</v>
+      </c>
       <c r="E18" s="2">
         <v>50458</v>
       </c>
+      <c r="F18" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E17</f>
+        <v>446</v>
+      </c>
+      <c r="G18" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>8.1008968609865484</v>
+      </c>
+      <c r="H18" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>8.1008968609865484</v>
+      </c>
       <c r="J18" s="1">
         <v>45139</v>
       </c>
@@ -945,16 +2366,32 @@
         <v>1.5109999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>45198</v>
       </c>
       <c r="C19" s="3">
         <v>38.51</v>
       </c>
+      <c r="D19" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>61.153880000000001</v>
+      </c>
       <c r="E19" s="2">
         <v>50991</v>
       </c>
+      <c r="F19" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E18</f>
+        <v>533</v>
+      </c>
+      <c r="G19" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.2251407129455911</v>
+      </c>
+      <c r="H19" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.2251407129455911</v>
+      </c>
       <c r="J19" s="1">
         <v>45155</v>
       </c>
@@ -962,16 +2399,32 @@
         <v>1.5109999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>45205</v>
       </c>
       <c r="C20" s="3">
         <v>38.840000000000003</v>
       </c>
+      <c r="D20" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>61.677920000000007</v>
+      </c>
       <c r="E20" s="2">
         <v>51593</v>
       </c>
+      <c r="F20" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E19</f>
+        <v>602</v>
+      </c>
+      <c r="G20" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.4518272425249172</v>
+      </c>
+      <c r="H20" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>6.4518272425249172</v>
+      </c>
       <c r="J20" s="1">
         <v>45167</v>
       </c>
@@ -979,16 +2432,32 @@
         <v>1.544</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>45213</v>
       </c>
       <c r="C21" s="3">
         <v>41.73</v>
       </c>
+      <c r="D21" s="6">
+        <f>INDEX(Table3[Bencin], MATCH(realna_poraba_cupra__2[[#This Row],[Datum]], Table3[Veljavnost], 1))*realna_poraba_cupra__2[[#This Row],[Litri]]</f>
+        <v>64.097279999999998</v>
+      </c>
       <c r="E21" s="2">
         <v>52176</v>
       </c>
+      <c r="F21" s="2">
+        <f>realna_poraba_cupra__2[[#This Row],[Števec]]-E20</f>
+        <v>583</v>
+      </c>
+      <c r="G21" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.1578044596912509</v>
+      </c>
+      <c r="H21" s="3">
+        <f>realna_poraba_cupra__2[[#This Row],[Litri]]/realna_poraba_cupra__2[[#This Row],[Prevoženo]]*100</f>
+        <v>7.1578044596912509</v>
+      </c>
       <c r="J21" s="1">
         <v>45181</v>
       </c>
@@ -996,7 +2465,7 @@
         <v>1.5509999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J22" s="1">
         <v>45195</v>
       </c>
@@ -1004,7 +2473,7 @@
         <v>1.5880000000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J23" s="1">
         <v>45209</v>
       </c>
@@ -1012,7 +2481,7 @@
         <v>1.536</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J24" s="1">
         <v>45223</v>
       </c>
@@ -1020,7 +2489,7 @@
         <v>1.536</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J25" s="1">
         <v>45237</v>
       </c>
@@ -1028,28 +2497,121 @@
         <v>1.534</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1789</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1850</v>
+      </c>
+      <c r="E29" s="9">
+        <v>2321</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1138</v>
+      </c>
+      <c r="G29" s="9">
+        <v>1986</v>
+      </c>
+      <c r="H29" s="9">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="3">
+        <v>6.643286586493633</v>
+      </c>
+      <c r="D30" s="3">
+        <v>6.7096452146904353</v>
+      </c>
+      <c r="E30" s="3">
+        <v>6.9488756233742244</v>
+      </c>
+      <c r="F30" s="3">
+        <v>6.909147776539081</v>
+      </c>
+      <c r="G30" s="3">
+        <v>7.5451560100243888</v>
+      </c>
+      <c r="H30" s="3">
+        <v>6.8048158511080841</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H4:H21">
+    <cfRule type="dataBar" priority="1">
+      <dataBar showValue="0">
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9B14FCA3-4D9F-4179-9E1B-F6AB205B5F86}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9B14FCA3-4D9F-4179-9E1B-F6AB205B5F86}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="min"/>
+              <x14:cfvo type="max"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H4:H21</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>